<commit_message>
some changes in list 6 and 7
</commit_message>
<xml_diff>
--- a/lista6/dane_double.xlsx
+++ b/lista6/dane_double.xlsx
@@ -48,8 +48,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -138,12 +139,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,16 +381,16 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>320</c:v>
@@ -420,46 +429,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.057</c:v>
+                  <c:v>0.06992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05612</c:v>
+                  <c:v>0.09076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13998</c:v>
+                  <c:v>0.09564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06664</c:v>
+                  <c:v>0.11334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.08862</c:v>
+                  <c:v>0.11806</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20746</c:v>
+                  <c:v>0.1758</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32512</c:v>
+                  <c:v>0.29024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97756</c:v>
+                  <c:v>0.9098</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.39148</c:v>
+                  <c:v>2.66556</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.34152</c:v>
+                  <c:v>10.12618</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40.06382</c:v>
+                  <c:v>39.64716</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>142.76498</c:v>
+                  <c:v>148.07838</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>550.38468</c:v>
+                  <c:v>577.5188</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2548.42502</c:v>
+                  <c:v>2342.22726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,25 +555,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1280</c:v>
@@ -597,46 +606,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.2537</c:v>
+                  <c:v>0.09902</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.06034</c:v>
+                  <c:v>0.12898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18184</c:v>
+                  <c:v>0.16076</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.06836</c:v>
+                  <c:v>0.18084</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28552</c:v>
+                  <c:v>0.23604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2719</c:v>
+                  <c:v>0.28768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.56142</c:v>
+                  <c:v>0.31536</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.43436</c:v>
+                  <c:v>0.75878</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.57588</c:v>
+                  <c:v>2.81892</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.94062</c:v>
+                  <c:v>11.95006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.73506</c:v>
+                  <c:v>38.576</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.66864</c:v>
+                  <c:v>149.7862</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>566.8619</c:v>
+                  <c:v>590.14656</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2431.4604</c:v>
+                  <c:v>2417.95612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,16 +738,16 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>640</c:v>
@@ -774,46 +783,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.0378</c:v>
+                  <c:v>0.03892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.04864</c:v>
+                  <c:v>0.05108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12658</c:v>
+                  <c:v>0.05994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0958</c:v>
+                  <c:v>0.09452</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11468</c:v>
+                  <c:v>0.09862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27662</c:v>
+                  <c:v>0.10188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27946</c:v>
+                  <c:v>0.2487</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83696</c:v>
+                  <c:v>0.80536</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.08622</c:v>
+                  <c:v>2.3749</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.11496</c:v>
+                  <c:v>8.8841</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.6783</c:v>
+                  <c:v>37.89766</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>136.89218</c:v>
+                  <c:v>159.97524</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>555.01372</c:v>
+                  <c:v>580.82538</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2201.03308</c:v>
+                  <c:v>2331.94736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -900,16 +909,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>160</c:v>
@@ -951,57 +960,57 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.02518</c:v>
+                  <c:v>0.01308</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03316</c:v>
+                  <c:v>0.0147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.02002</c:v>
+                  <c:v>0.01676</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.07854</c:v>
+                  <c:v>0.01744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13406</c:v>
+                  <c:v>0.0497</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.256</c:v>
+                  <c:v>0.08066</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26952</c:v>
+                  <c:v>0.24792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76932</c:v>
+                  <c:v>0.8152</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.70852</c:v>
+                  <c:v>3.64846</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.44596</c:v>
+                  <c:v>13.28056</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.35208</c:v>
+                  <c:v>53.3205</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>192.8379</c:v>
+                  <c:v>207.8004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>730.39316</c:v>
+                  <c:v>774.8528</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4143.72242</c:v>
+                  <c:v>2378.4486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51175158"/>
-        <c:axId val="40701634"/>
+        <c:axId val="19909554"/>
+        <c:axId val="39042378"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51175158"/>
+        <c:axId val="19909554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90000"/>
@@ -1088,12 +1097,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40701634"/>
+        <c:crossAx val="39042378"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40701634"/>
+        <c:axId val="39042378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1178,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51175158"/>
+        <c:crossAx val="19909554"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1233,9 +1242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>523080</xdr:colOff>
+      <xdr:colOff>522720</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1244,7 +1253,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4042440" y="6348600"/>
-        <a:ext cx="7053480" cy="3614400"/>
+        <a:ext cx="7053120" cy="3614040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1468,642 +1477,643 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>0.06992</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>0.05612</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1" t="n">
+        <v>0.09076</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.09564</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.13998</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B5" s="1" t="n">
+        <v>0.11334</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.11806</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0.06664</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B7" s="1" t="n">
+        <v>0.1758</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0.29024</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0.9098</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2.66556</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>10.12618</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>39.64716</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>148.07838</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>577.5188</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2342.22726</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>81920</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>0.09902</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0.12898</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.08862</v>
-      </c>
-      <c r="C6" s="0" t="n">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>0.16076</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0.18084</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>0.23604</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>0.28768</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>0.31536</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>0.75878</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>2.81892</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>11.95006</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>38.576</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>149.7862</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>590.14656</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>2417.95612</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>81920</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0.03892</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>0.05108</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0.05994</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0.09452</v>
+      </c>
+      <c r="C33" s="1" t="n">
         <v>160</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.20746</v>
-      </c>
-      <c r="C7" s="0" t="n">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>0.09862</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>320</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.32512</v>
-      </c>
-      <c r="C8" s="0" t="n">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>0.10188</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0.2487</v>
+      </c>
+      <c r="C36" s="1" t="n">
         <v>640</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>0.97756</v>
-      </c>
-      <c r="C9" s="0" t="n">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0.80536</v>
+      </c>
+      <c r="C37" s="1" t="n">
         <v>1280</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>3.39148</v>
-      </c>
-      <c r="C10" s="0" t="n">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>2.3749</v>
+      </c>
+      <c r="C38" s="1" t="n">
         <v>2560</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>12.34152</v>
-      </c>
-      <c r="C11" s="0" t="n">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>8.8841</v>
+      </c>
+      <c r="C39" s="1" t="n">
         <v>5120</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>40.06382</v>
-      </c>
-      <c r="C12" s="0" t="n">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>37.89766</v>
+      </c>
+      <c r="C40" s="1" t="n">
         <v>10240</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>142.76498</v>
-      </c>
-      <c r="C13" s="0" t="n">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>159.97524</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>20480</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>550.38468</v>
-      </c>
-      <c r="C14" s="0" t="n">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>580.82538</v>
+      </c>
+      <c r="C42" s="1" t="n">
         <v>40960</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>2548.42502</v>
-      </c>
-      <c r="C15" s="0" t="n">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>2331.94736</v>
+      </c>
+      <c r="C43" s="1" t="n">
         <v>81920</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>0.2537</v>
-      </c>
-      <c r="C16" s="0" t="n">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>0.01308</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="C45" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0.06034</v>
-      </c>
-      <c r="C17" s="0" t="n">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>0.01676</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>0.01744</v>
+      </c>
+      <c r="C47" s="1" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0.18184</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0.06836</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>0.28552</v>
-      </c>
-      <c r="C20" s="0" t="n">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>0.0497</v>
+      </c>
+      <c r="C48" s="1" t="n">
         <v>160</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>0.2719</v>
-      </c>
-      <c r="C21" s="0" t="n">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>0.08066</v>
+      </c>
+      <c r="C49" s="1" t="n">
         <v>320</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>1.56142</v>
-      </c>
-      <c r="C22" s="0" t="n">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>0.24792</v>
+      </c>
+      <c r="C50" s="1" t="n">
         <v>640</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>1.43436</v>
-      </c>
-      <c r="C23" s="0" t="n">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>0.8152</v>
+      </c>
+      <c r="C51" s="1" t="n">
         <v>1280</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>3.57588</v>
-      </c>
-      <c r="C24" s="0" t="n">
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>3.64846</v>
+      </c>
+      <c r="C52" s="1" t="n">
         <v>2560</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>10.94062</v>
-      </c>
-      <c r="C25" s="0" t="n">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>13.28056</v>
+      </c>
+      <c r="C53" s="1" t="n">
         <v>5120</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>42.73506</v>
-      </c>
-      <c r="C26" s="0" t="n">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>53.3205</v>
+      </c>
+      <c r="C54" s="1" t="n">
         <v>10240</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>143.66864</v>
-      </c>
-      <c r="C27" s="0" t="n">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>207.8004</v>
+      </c>
+      <c r="C55" s="1" t="n">
         <v>20480</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>566.8619</v>
-      </c>
-      <c r="C28" s="0" t="n">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>774.8528</v>
+      </c>
+      <c r="C56" s="1" t="n">
         <v>40960</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>2431.4604</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>81920</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0.0378</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>0.04864</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>0.12658</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>0.0958</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>0.11468</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>0.27662</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0.27946</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>0.83696</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>3.08622</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>10.11496</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>36.6783</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>136.89218</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>20480</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>555.01372</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>40960</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>2201.03308</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>81920</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>0.02518</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>0.03316</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>0.02002</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>0.07854</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>0.13406</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>0.256</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>0.26952</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>0.76932</v>
-      </c>
-      <c r="C51" s="0" t="n">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>3.70852</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>11.44596</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>55.35208</v>
-      </c>
-      <c r="C54" s="0" t="n">
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>192.8379</v>
-      </c>
-      <c r="C55" s="0" t="n">
-        <v>20480</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>730.39316</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>40960</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>4143.72242</v>
-      </c>
-      <c r="C57" s="0" t="n">
+      <c r="B57" s="1" t="n">
+        <v>2378.4486</v>
+      </c>
+      <c r="C57" s="1" t="n">
         <v>81920</v>
       </c>
     </row>

</xml_diff>